<commit_message>
Both: Changed chat messages data sentences
</commit_message>
<xml_diff>
--- a/data-senteces.xlsx
+++ b/data-senteces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CursedKingdom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0580F8-49A3-47EB-BB71-1B4FE76EFB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607A80A9-39F8-4659-8036-6F8DDA074F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33915" yWindow="3870" windowWidth="21600" windowHeight="11385" xr2:uid="{4548776F-D2DA-41AE-8E15-FA17EE5DDF1B}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:AC110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>